<commit_message>
template for users load now xlsx
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="3AXwzqba+LpoikTurMEIYi1PxsFbYRS5GwBSpo9IKw0B/TIGIxYwwy/6zFWj+MOmIC6MDs9axiedack8WouMSw==" workbookSaltValue="1pKrQ9UpiE3nnBZCmDVSmA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$241</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="489">
   <si>
     <t>CI</t>
   </si>
@@ -38,16 +43,1462 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>sex</t>
   </si>
   <si>
+    <t>country</t>
+  </si>
+  <si>
     <t>country_id</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>Afganistán</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Alemania</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>Antártida</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>Antigua y Barbuda</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>Antillas Holandesas</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Arabia Saudí</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>Argelia</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>ARY Macedonia</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Azerbaiyán</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>BH</t>
+  </si>
+  <si>
+    <t>Bahréin</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Bélgica</t>
+  </si>
+  <si>
+    <t>BZ</t>
+  </si>
+  <si>
+    <t>Belice</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>Bermudas</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>Bhután</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>Bielorrusia</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Bosnia y Herzegovina</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>Botsuana</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>Brunéi</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>Camboya</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Camerún</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Canadá</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>Chipre</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Ciudad del Vaticano</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>Comoras</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
+    <t>Corea del Norte</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>Corea del Sur</t>
+  </si>
+  <si>
+    <t>Costa de Marfil</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Croacia</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Dinamarca</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>Egipto</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>Emiratos Árabes Unidos</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Eslovaquia</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Eslovenia</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Estados Unidos</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Etiopía</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>Filipinas</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Finlandia</t>
+  </si>
+  <si>
+    <t>FJ</t>
+  </si>
+  <si>
+    <t>Fiyi</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Francia</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Gabón</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>Granada</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Grecia</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>Groenlandia</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>Guadalupe</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>Guayana Francesa</t>
+  </si>
+  <si>
+    <t>GN</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>Guinea Ecuatorial</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>Haití</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>Hungría</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Irán</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Irlanda</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>Isla Bouvet</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>Isla de Navidad</t>
+  </si>
+  <si>
+    <t>NF</t>
+  </si>
+  <si>
+    <t>Isla Norfolk</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>Islandia</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>Islas Caimán</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Islas Cocos</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>Islas Cook</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>Islas Feroe</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>Islas Georgias del Sur y Sandwich del Sur</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>Islas Gland</t>
+  </si>
+  <si>
+    <t>HM</t>
+  </si>
+  <si>
+    <t>Islas Heard y McDonald</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>Islas Malvinas</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Islas Marianas del Norte</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>Islas Marshall</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>Islas Pitcairn</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Islas Salomón</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Islas Turcas y Caicos</t>
+  </si>
+  <si>
+    <t>UM</t>
+  </si>
+  <si>
+    <t>Islas ultramarinas de Estados Unidos</t>
+  </si>
+  <si>
+    <t>VG</t>
+  </si>
+  <si>
+    <t>Islas Vírgenes Británicas</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>Islas Vírgenes de los Estados Unidos</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>JM</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Japón</t>
+  </si>
+  <si>
+    <t>JO</t>
+  </si>
+  <si>
+    <t>Jordania</t>
+  </si>
+  <si>
+    <t>KZ</t>
+  </si>
+  <si>
+    <t>Kazajstán</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>Kenia</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>Kirguistán</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>Letonia</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>Líbano</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>Libia</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>Lituania</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>Luxemburgo</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>Malasia</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>Maldivas</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Malí</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Marruecos</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>Martinica</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>YT</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Moldavia</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Mónaco</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Montserrat</t>
+  </si>
+  <si>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Níger</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Noruega</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>Nueva Caledonia</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>Nueva Zelanda</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>Omán</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>Países Bajos</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Pakistán</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Palestina</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Panamá</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>Papúa Nueva Guinea</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Perú</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>Polinesia Francesa</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>Polonia</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>Reino Unido</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>República Centroafricana</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>República Checa</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>República Democrática del Congo</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>República Dominicana</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>Reunión</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>Ruanda</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>Rumania</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>Rusia</t>
+  </si>
+  <si>
+    <t>EH</t>
+  </si>
+  <si>
+    <t>Sahara Occidental</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Samoa Americana</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>San Cristóbal y Nevis</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>San Pedro y Miquelón</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>San Vicente y las Granadinas</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>Santa Helena</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Santa Lucía</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Santo Tomé y Príncipe</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Serbia y Montenegro</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Sierra Leona</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Singapur</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>Siria</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>Suazilandia</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>Sudáfrica</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Sudán</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Suecia</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Suiza</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Surinam</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>Svalbard y Jan Mayen</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Tailandia</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>Taiwán</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>Tayikistán</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>Territorio Británico del Océano Índico</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>Territorios Australes Franceses</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>Timor Oriental</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Trinidad y Tobago</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Túnez</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>Turkmenistán</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Turquía</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>Ucrania</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>UY</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>UZ</t>
+  </si>
+  <si>
+    <t>Uzbekistán</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>Wallis y Futuna</t>
+  </si>
+  <si>
+    <t>YE</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>Yibuti</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>Zimbabue</t>
   </si>
 </sst>
 </file>
@@ -60,7 +1511,7 @@
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,11 +1520,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,7 +1970,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -533,16 +1989,13 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -551,124 +2004,142 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -718,6 +2189,7 @@
     <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="49"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -940,6 +2412,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1200,39 +2679,2760 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="11" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3"/>
+    <col min="3" max="3" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.287037037037" style="3" customWidth="1"/>
+    <col min="5" max="6" width="10" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Ls44ZquHRmGxO4RH86y0kMhaJcffuWFz2t5djTFVWcfJ1MHtMBU3YZs95AIMT1eH5fK2kunaMkPu4yJRtuHVhA==" saltValue="w6GsrLb0N8tOXICf7Gezjg==" spinCount="100000" sheet="1" objects="1"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E2000">
+      <formula1>Sheet1!$E$2:$E$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F2000">
+      <formula1>Sheet1!$C$2:$C$241</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E241"/>
+  <sheetViews>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <cols>
+    <col min="3" max="3" width="19.4259259259259" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>138</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>48</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>53</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>54</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>62</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>64</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>65</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>67</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>68</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>2</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>70</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>71</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>74</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>75</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>76</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>77</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>78</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>79</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>80</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>82</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>83</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>84</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>86</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>87</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>88</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>89</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>90</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>91</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>92</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>94</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>95</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>96</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>97</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>98</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>99</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>100</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>101</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>102</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>103</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>104</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>105</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>106</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>107</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>109</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>110</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>111</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
+        <v>112</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
+        <v>113</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
+        <v>114</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
+        <v>115</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1">
+        <v>116</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1">
+        <v>39</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
+        <v>56</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1">
+        <v>168</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1">
+        <v>117</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1">
+        <v>46</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1">
+        <v>58</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1">
+        <v>63</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1">
+        <v>85</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1">
+        <v>93</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1">
+        <v>9</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1">
+        <v>108</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1">
+        <v>145</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1">
+        <v>146</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1">
+        <v>148</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1">
+        <v>181</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1">
+        <v>193</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1">
+        <v>230</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1">
+        <v>81</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1">
+        <v>241</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1">
+        <v>242</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1">
+        <v>118</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="1">
+        <v>119</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1">
+        <v>120</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1">
+        <v>121</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1">
+        <v>122</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1">
+        <v>123</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1">
+        <v>124</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1">
+        <v>125</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1">
+        <v>126</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1">
+        <v>127</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1">
+        <v>128</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="1">
+        <v>129</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1">
+        <v>130</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="1">
+        <v>131</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="1">
+        <v>132</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="1">
+        <v>133</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1">
+        <v>134</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="1">
+        <v>135</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="1">
+        <v>136</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="1">
+        <v>137</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1">
+        <v>139</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1">
+        <v>140</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1">
+        <v>141</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1">
+        <v>142</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1">
+        <v>143</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1">
+        <v>144</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1">
+        <v>147</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="1">
+        <v>149</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1">
+        <v>150</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1">
+        <v>151</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="1">
+        <v>152</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="1">
+        <v>153</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="1">
+        <v>154</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="1">
+        <v>155</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="1">
+        <v>156</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="1">
+        <v>157</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="1">
+        <v>158</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="1">
+        <v>159</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="1">
+        <v>160</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="1">
+        <v>161</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1">
+        <v>162</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="1">
+        <v>163</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="1">
+        <v>164</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="1">
+        <v>165</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="1">
+        <v>166</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="1">
+        <v>167</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="1">
+        <v>169</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="1">
+        <v>170</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="1">
+        <v>171</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="1">
+        <v>172</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="1">
+        <v>173</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="1">
+        <v>174</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="1">
+        <v>175</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="1">
+        <v>176</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="1">
+        <v>177</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="1">
+        <v>178</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="1">
+        <v>179</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="1">
+        <v>180</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="1">
+        <v>182</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="1">
+        <v>183</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="1">
+        <v>184</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="1">
+        <v>185</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="1">
+        <v>186</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="1">
+        <v>187</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="1">
+        <v>50</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="1">
+        <v>52</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="1">
+        <v>61</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="1">
+        <v>72</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="1">
+        <v>188</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="1">
+        <v>189</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="1">
+        <v>190</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="1">
+        <v>191</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="1">
+        <v>192</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="1">
+        <v>194</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="1">
+        <v>195</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="1">
+        <v>196</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="1">
+        <v>197</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="1">
+        <v>198</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="1">
+        <v>199</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="1">
+        <v>200</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="1">
+        <v>201</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="1">
+        <v>202</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1">
+        <v>203</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="1">
+        <v>204</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="1">
+        <v>205</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="1">
+        <v>206</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="1">
+        <v>207</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="1">
+        <v>208</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1">
+        <v>209</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="1">
+        <v>210</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="1">
+        <v>211</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="1">
+        <v>212</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="1">
+        <v>213</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="1">
+        <v>214</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="1">
+        <v>215</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="1">
+        <v>216</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="1">
+        <v>217</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="1">
+        <v>218</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="1">
+        <v>219</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="1">
+        <v>220</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="1">
+        <v>221</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="1">
+        <v>222</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="1">
+        <v>223</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="1">
+        <v>224</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="1">
+        <v>225</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="1">
+        <v>226</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="1">
+        <v>227</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="1">
+        <v>228</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="1">
+        <v>229</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="1">
+        <v>231</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="1">
+        <v>232</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="1">
+        <v>233</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="1">
+        <v>234</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="1">
+        <v>235</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="1">
+        <v>236</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="1">
+        <v>237</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="1">
+        <v>238</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="1">
+        <v>239</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="1">
+        <v>240</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="1">
+        <v>243</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="1">
+        <v>244</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="1">
+        <v>245</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="1">
+        <v>246</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="1">
+        <v>247</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C241" etc:filterBottomFollowUsedRange="0">
+    <sortState ref="A1:C241">
+      <sortCondition ref="C1"/>
+    </sortState>
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
+  <rangeList sheetStid="1" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="2" master="" otherUserPermission="visible"/>
+</allowEditUser>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>